<commit_message>
added TODO ID, fixed bugs, learned about vbs. How antequated it is...
</commit_message>
<xml_diff>
--- a/Calibration_TMA_SOP Schedule_Master Form 101359 TODO.xlsx
+++ b/Calibration_TMA_SOP Schedule_Master Form 101359 TODO.xlsx
@@ -27,7 +27,6 @@
     <sheet name="BiodieselGC Room" sheetId="4" r:id="rId13"/>
     <sheet name="Specifications" sheetId="3" r:id="rId14"/>
     <sheet name="Items for multiple tests" sheetId="2" r:id="rId15"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId16"/>
   </sheets>
   <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
@@ -39,7 +38,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="33">
+  <si>
+    <t xml:space="preserve">Master Form 101359 Calibration, Verification, Standardization Schedule </t>
+  </si>
   <si>
     <t>Location</t>
   </si>
@@ -71,6 +73,9 @@
     <t>TODO ID</t>
   </si>
   <si>
+    <t xml:space="preserve">Calibration, Verification, Standardization Schedule </t>
+  </si>
+  <si>
     <t>Current ASTM Version</t>
   </si>
   <si>
@@ -105,6 +110,12 @@
   </si>
   <si>
     <t>Calibration due date</t>
+  </si>
+  <si>
+    <t>Section J</t>
+  </si>
+  <si>
+    <t>NOT DATA</t>
   </si>
   <si>
     <t>Thermometer</t>
@@ -132,9 +143,33 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -149,10 +184,36 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -161,13 +222,256 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="19">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -477,741 +781,1310 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.109375" customWidth="1"/>
+    <col min="2" max="3" width="15.44140625" customWidth="1"/>
+    <col min="4" max="5" width="14.44140625" customWidth="1"/>
+    <col min="6" max="6" width="15.44140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" t="s">
+    <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="F2" t="s">
-        <v>24</v>
-      </c>
       <c r="G2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:G1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:O2"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.44140625" customWidth="1"/>
+    <col min="2" max="2" width="20.109375" customWidth="1"/>
+    <col min="3" max="3" width="11.44140625" customWidth="1"/>
+    <col min="4" max="4" width="20.109375" customWidth="1"/>
+    <col min="5" max="6" width="18.44140625" customWidth="1"/>
+    <col min="7" max="7" width="18" customWidth="1"/>
+    <col min="8" max="8" width="14.44140625" customWidth="1"/>
+    <col min="9" max="9" width="18" customWidth="1"/>
+    <col min="10" max="10" width="20.109375" customWidth="1"/>
+    <col min="11" max="11" width="16.109375" customWidth="1"/>
+    <col min="12" max="12" width="16" customWidth="1"/>
+    <col min="13" max="13" width="26.109375" customWidth="1"/>
+    <col min="14" max="14" width="47.44140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="1" spans="1:15" ht="79.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
+    </row>
+    <row r="2" spans="1:15" ht="79.95" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" t="s">
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" t="s">
+      <c r="E2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G2" t="s">
+      <c r="F2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H2" t="s">
+      <c r="G2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I2" t="s">
+      <c r="H2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J2" t="s">
-        <v>7</v>
-      </c>
-      <c r="K2" t="s">
-        <v>11</v>
-      </c>
-      <c r="L2" t="s">
+      <c r="I2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="N2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="M2" t="s">
-        <v>13</v>
-      </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>10</v>
       </c>
-      <c r="O2" t="s">
-        <v>9</v>
-      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:O1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="I2">
+    <cfRule type="timePeriod" dxfId="12" priority="1" timePeriod="nextWeek">
+      <formula>AND(ROUNDDOWN(I2,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(I2,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
+    </cfRule>
+    <cfRule type="timePeriod" dxfId="11" priority="2" timePeriod="thisWeek">
+      <formula>AND(TODAY()-ROUNDDOWN(I2,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(I2,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:O2"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.44140625" customWidth="1"/>
+    <col min="2" max="2" width="22.109375" customWidth="1"/>
+    <col min="3" max="3" width="9.44140625" customWidth="1"/>
+    <col min="4" max="4" width="20.109375" customWidth="1"/>
+    <col min="5" max="5" width="18.44140625" customWidth="1"/>
+    <col min="6" max="6" width="22.44140625" customWidth="1"/>
+    <col min="7" max="7" width="18" customWidth="1"/>
+    <col min="8" max="8" width="14.44140625" customWidth="1"/>
+    <col min="9" max="9" width="18" customWidth="1"/>
+    <col min="10" max="10" width="20.109375" customWidth="1"/>
+    <col min="11" max="12" width="16.109375" customWidth="1"/>
+    <col min="13" max="13" width="18" customWidth="1"/>
+    <col min="14" max="14" width="22.109375" customWidth="1"/>
+    <col min="15" max="15" width="11.109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="1" spans="1:15" ht="79.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
+    </row>
+    <row r="2" spans="1:15" s="8" customFormat="1" ht="79.95" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" t="s">
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" t="s">
+      <c r="E2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G2" t="s">
+      <c r="F2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H2" t="s">
+      <c r="G2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I2" t="s">
+      <c r="H2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J2" t="s">
-        <v>7</v>
-      </c>
-      <c r="K2" t="s">
-        <v>11</v>
-      </c>
-      <c r="L2" t="s">
+      <c r="I2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="N2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="M2" t="s">
-        <v>13</v>
-      </c>
-      <c r="N2" t="s">
+      <c r="O2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="O2" t="s">
-        <v>9</v>
-      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:O1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="I2">
+    <cfRule type="timePeriod" dxfId="10" priority="2" timePeriod="nextWeek">
+      <formula>AND(ROUNDDOWN(I2,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(I2,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
+    </cfRule>
+    <cfRule type="timePeriod" dxfId="9" priority="3" timePeriod="thisWeek">
+      <formula>AND(TODAY()-ROUNDDOWN(I2,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(I2,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I2">
+    <cfRule type="timePeriod" dxfId="8" priority="1" timePeriod="nextMonth">
+      <formula>AND(MONTH(I2)=MONTH(EDATE(TODAY(),0+1)),YEAR(I2)=YEAR(EDATE(TODAY(),0+1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:O2"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.44140625" customWidth="1"/>
+    <col min="2" max="2" width="24.44140625" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" customWidth="1"/>
+    <col min="4" max="4" width="31.44140625" customWidth="1"/>
+    <col min="5" max="5" width="20.109375" customWidth="1"/>
+    <col min="6" max="6" width="29.77734375" customWidth="1"/>
+    <col min="7" max="7" width="18" customWidth="1"/>
+    <col min="8" max="8" width="18.109375" customWidth="1"/>
+    <col min="9" max="9" width="18" customWidth="1"/>
+    <col min="10" max="10" width="20.109375" customWidth="1"/>
+    <col min="11" max="12" width="16.109375" customWidth="1"/>
+    <col min="13" max="13" width="19.44140625" customWidth="1"/>
+    <col min="14" max="14" width="20.44140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="1" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
+    </row>
+    <row r="2" spans="1:15" ht="70.2" x14ac:dyDescent="0.45">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" t="s">
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" t="s">
+      <c r="E2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G2" t="s">
+      <c r="F2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H2" t="s">
+      <c r="G2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I2" t="s">
+      <c r="H2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J2" t="s">
-        <v>7</v>
-      </c>
-      <c r="K2" t="s">
-        <v>11</v>
-      </c>
-      <c r="L2" t="s">
+      <c r="I2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="N2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="M2" t="s">
-        <v>13</v>
-      </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>10</v>
       </c>
-      <c r="O2" t="s">
-        <v>9</v>
-      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:O1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="I2">
+    <cfRule type="timePeriod" dxfId="7" priority="1" timePeriod="nextWeek">
+      <formula>AND(ROUNDDOWN(I2,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(I2,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
+    </cfRule>
+    <cfRule type="timePeriod" dxfId="6" priority="2" timePeriod="thisWeek">
+      <formula>AND(TODAY()-ROUNDDOWN(I2,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(I2,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:O2"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.109375" customWidth="1"/>
+    <col min="2" max="2" width="22" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" customWidth="1"/>
+    <col min="4" max="4" width="34.44140625" customWidth="1"/>
+    <col min="5" max="5" width="20.44140625" customWidth="1"/>
+    <col min="6" max="6" width="23.77734375" customWidth="1"/>
+    <col min="7" max="7" width="22.109375" customWidth="1"/>
+    <col min="8" max="8" width="18.109375" customWidth="1"/>
+    <col min="9" max="9" width="21.44140625" customWidth="1"/>
+    <col min="10" max="12" width="16.44140625" customWidth="1"/>
+    <col min="13" max="13" width="20.109375" customWidth="1"/>
+    <col min="14" max="14" width="17.44140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="1" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+    </row>
+    <row r="2" spans="1:15" ht="70.2" x14ac:dyDescent="0.45">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" t="s">
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" t="s">
+      <c r="E2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G2" t="s">
+      <c r="F2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H2" t="s">
+      <c r="G2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I2" t="s">
+      <c r="H2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J2" t="s">
-        <v>7</v>
-      </c>
-      <c r="K2" t="s">
-        <v>11</v>
-      </c>
-      <c r="L2" t="s">
+      <c r="I2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="N2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="M2" t="s">
-        <v>13</v>
-      </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>10</v>
       </c>
-      <c r="O2" t="s">
-        <v>9</v>
-      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:J1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="I1">
+    <cfRule type="timePeriod" dxfId="5" priority="3" timePeriod="nextWeek">
+      <formula>AND(ROUNDDOWN(I1,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(I1,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
+    </cfRule>
+    <cfRule type="timePeriod" dxfId="4" priority="4" timePeriod="thisWeek">
+      <formula>AND(TODAY()-ROUNDDOWN(I1,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(I1,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I2">
+    <cfRule type="timePeriod" dxfId="3" priority="1" timePeriod="nextWeek">
+      <formula>AND(ROUNDDOWN(I2,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(I2,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
+    </cfRule>
+    <cfRule type="timePeriod" dxfId="2" priority="2" timePeriod="thisWeek">
+      <formula>AND(TODAY()-ROUNDDOWN(I2,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(I2,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.44140625" customWidth="1"/>
+    <col min="2" max="2" width="23.44140625" customWidth="1"/>
+    <col min="3" max="3" width="17.109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+    </row>
+    <row r="2" spans="1:9" ht="70.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:I1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="H1">
+    <cfRule type="timePeriod" dxfId="1" priority="1" timePeriod="nextWeek">
+      <formula>AND(ROUNDDOWN(H1,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(H1,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
+    </cfRule>
+    <cfRule type="timePeriod" dxfId="0" priority="2" timePeriod="thisWeek">
+      <formula>AND(TODAY()-ROUNDDOWN(H1,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(H1,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:K2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.44140625" customWidth="1"/>
+    <col min="2" max="2" width="19" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" customWidth="1"/>
+    <col min="4" max="4" width="20.109375" customWidth="1"/>
+    <col min="5" max="6" width="18.44140625" customWidth="1"/>
+    <col min="7" max="7" width="18" customWidth="1"/>
+    <col min="8" max="8" width="15.109375" customWidth="1"/>
+    <col min="9" max="9" width="18" customWidth="1"/>
+    <col min="10" max="10" width="20.109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="1" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+    </row>
+    <row r="2" spans="1:11" ht="58.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" t="s">
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" t="s">
+      <c r="E2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G2" t="s">
+      <c r="F2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H2" t="s">
+      <c r="G2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I2" t="s">
+      <c r="H2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J2" t="s">
-        <v>7</v>
+      <c r="I2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="K2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <mergeCells count="1">
+    <mergeCell ref="A1:J1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.44140625" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="15.109375" customWidth="1"/>
+    <col min="4" max="4" width="12" customWidth="1"/>
+    <col min="5" max="5" width="19.109375" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
+    <row r="1" spans="1:10" ht="79.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+    </row>
+    <row r="2" spans="1:10" ht="79.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19.44140625" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" customWidth="1"/>
+    <col min="3" max="3" width="15.44140625" customWidth="1"/>
+    <col min="4" max="4" width="16.109375" customWidth="1"/>
+    <col min="5" max="5" width="23.77734375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
+    <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:O2"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.44140625" customWidth="1"/>
+    <col min="2" max="2" width="17.44140625" customWidth="1"/>
+    <col min="3" max="3" width="9.44140625" customWidth="1"/>
+    <col min="4" max="4" width="20.109375" customWidth="1"/>
+    <col min="5" max="6" width="18.44140625" customWidth="1"/>
+    <col min="7" max="7" width="18" customWidth="1"/>
+    <col min="8" max="8" width="15.109375" customWidth="1"/>
+    <col min="9" max="9" width="18" customWidth="1"/>
+    <col min="10" max="10" width="20.109375" customWidth="1"/>
+    <col min="11" max="12" width="13" customWidth="1"/>
+    <col min="13" max="13" width="17.44140625" customWidth="1"/>
+    <col min="14" max="14" width="22.44140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="1" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
+    </row>
+    <row r="2" spans="1:15" ht="70.2" x14ac:dyDescent="0.45">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" t="s">
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" t="s">
+      <c r="E2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G2" t="s">
+      <c r="F2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H2" t="s">
+      <c r="G2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I2" t="s">
+      <c r="H2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J2" t="s">
-        <v>7</v>
-      </c>
-      <c r="K2" t="s">
-        <v>11</v>
-      </c>
-      <c r="L2" t="s">
+      <c r="I2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="N2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="M2" t="s">
-        <v>13</v>
-      </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>10</v>
       </c>
-      <c r="O2" t="s">
-        <v>9</v>
-      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:O1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="22.109375" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" customWidth="1"/>
+    <col min="3" max="3" width="14.44140625" customWidth="1"/>
+    <col min="4" max="4" width="38.109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F2" t="s">
-        <v>9</v>
+    <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+    </row>
+    <row r="2" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:J1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="I1">
+    <cfRule type="timePeriod" dxfId="18" priority="1" timePeriod="nextWeek">
+      <formula>AND(ROUNDDOWN(I1,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(I1,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
+    </cfRule>
+    <cfRule type="timePeriod" dxfId="17" priority="2" timePeriod="thisWeek">
+      <formula>AND(TODAY()-ROUNDDOWN(I1,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(I1,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:I2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="7.109375" customWidth="1"/>
+    <col min="2" max="2" width="7.44140625" customWidth="1"/>
+    <col min="3" max="3" width="13.109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="9"/>
+    </row>
+    <row r="2" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>20</v>
       </c>
       <c r="E2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" t="s">
-        <v>20</v>
+        <v>21</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>22</v>
       </c>
       <c r="G2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" t="s">
         <v>21</v>
       </c>
-      <c r="I2" t="s">
-        <v>9</v>
+      <c r="H2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:J1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:P2"/>
+  <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.44140625" customWidth="1"/>
+    <col min="2" max="2" width="17.44140625" customWidth="1"/>
+    <col min="3" max="3" width="9.44140625" customWidth="1"/>
+    <col min="4" max="4" width="20.109375" customWidth="1"/>
+    <col min="5" max="5" width="20.44140625" customWidth="1"/>
+    <col min="6" max="6" width="22.109375" customWidth="1"/>
+    <col min="7" max="7" width="18" customWidth="1"/>
+    <col min="8" max="8" width="14.44140625" customWidth="1"/>
+    <col min="9" max="9" width="18" customWidth="1"/>
+    <col min="10" max="10" width="20.109375" customWidth="1"/>
+    <col min="11" max="12" width="14.44140625" customWidth="1"/>
+    <col min="13" max="13" width="22.44140625" customWidth="1"/>
+    <col min="14" max="14" width="17.109375" customWidth="1"/>
+    <col min="15" max="15" width="17.44140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="1" spans="1:16" ht="79.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
+      <c r="P1" s="17"/>
+    </row>
+    <row r="2" spans="1:16" ht="79.95" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" t="s">
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" t="s">
+      <c r="E2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G2" t="s">
+      <c r="F2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H2" t="s">
+      <c r="G2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I2" t="s">
+      <c r="H2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J2" t="s">
-        <v>7</v>
-      </c>
-      <c r="K2" t="s">
-        <v>11</v>
-      </c>
-      <c r="L2" t="s">
+      <c r="I2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="N2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="M2" t="s">
-        <v>13</v>
-      </c>
-      <c r="N2" t="s">
+      <c r="O2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="P2" t="s">
         <v>10</v>
       </c>
-      <c r="O2" t="s">
-        <v>14</v>
-      </c>
-      <c r="P2" t="s">
-        <v>9</v>
-      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:P1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="I2">
+    <cfRule type="timePeriod" dxfId="16" priority="1" timePeriod="nextWeek">
+      <formula>AND(ROUNDDOWN(I2,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(I2,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
+    </cfRule>
+    <cfRule type="timePeriod" dxfId="15" priority="2" timePeriod="thisWeek">
+      <formula>AND(TODAY()-ROUNDDOWN(I2,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(I2,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:O2"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.44140625" customWidth="1"/>
+    <col min="2" max="2" width="26.33203125" customWidth="1"/>
+    <col min="3" max="3" width="13.109375" customWidth="1"/>
+    <col min="4" max="4" width="20.109375" customWidth="1"/>
+    <col min="5" max="5" width="18.44140625" customWidth="1"/>
+    <col min="6" max="6" width="24.6640625" customWidth="1"/>
+    <col min="7" max="7" width="18" customWidth="1"/>
+    <col min="8" max="8" width="15" customWidth="1"/>
+    <col min="9" max="9" width="18" customWidth="1"/>
+    <col min="10" max="10" width="20.109375" customWidth="1"/>
+    <col min="11" max="12" width="16.109375" customWidth="1"/>
+    <col min="13" max="13" width="21" customWidth="1"/>
+    <col min="14" max="14" width="29.44140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="1" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
+    </row>
+    <row r="2" spans="1:15" ht="70.2" x14ac:dyDescent="0.45">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" t="s">
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" t="s">
+      <c r="E2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G2" t="s">
+      <c r="F2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H2" t="s">
+      <c r="G2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I2" t="s">
+      <c r="H2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J2" t="s">
-        <v>7</v>
-      </c>
-      <c r="K2" t="s">
-        <v>11</v>
-      </c>
-      <c r="L2" t="s">
+      <c r="I2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="N2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="M2" t="s">
-        <v>13</v>
-      </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>10</v>
       </c>
-      <c r="O2" t="s">
-        <v>9</v>
-      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:O1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:O2"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19.44140625" customWidth="1"/>
+    <col min="2" max="3" width="17.109375" customWidth="1"/>
+    <col min="4" max="4" width="20.109375" customWidth="1"/>
+    <col min="5" max="5" width="16.44140625" customWidth="1"/>
+    <col min="6" max="6" width="18.44140625" customWidth="1"/>
+    <col min="7" max="7" width="17.44140625" customWidth="1"/>
+    <col min="8" max="8" width="15.44140625" customWidth="1"/>
+    <col min="9" max="10" width="17.109375" customWidth="1"/>
+    <col min="11" max="12" width="13.44140625" customWidth="1"/>
+    <col min="13" max="13" width="15.109375" customWidth="1"/>
+    <col min="14" max="14" width="12.109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="1" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
+    </row>
+    <row r="2" spans="1:15" ht="70.2" x14ac:dyDescent="0.45">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" t="s">
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" t="s">
+      <c r="E2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G2" t="s">
+      <c r="F2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H2" t="s">
+      <c r="G2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I2" t="s">
+      <c r="H2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J2" t="s">
-        <v>7</v>
-      </c>
-      <c r="K2" t="s">
-        <v>11</v>
-      </c>
-      <c r="L2" t="s">
+      <c r="I2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="N2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="M2" t="s">
-        <v>13</v>
-      </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>10</v>
       </c>
-      <c r="O2" t="s">
-        <v>9</v>
-      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:O1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="I2">
+    <cfRule type="timePeriod" dxfId="14" priority="1" timePeriod="nextWeek">
+      <formula>AND(ROUNDDOWN(I2,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(I2,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
+    </cfRule>
+    <cfRule type="timePeriod" dxfId="13" priority="2" timePeriod="thisWeek">
+      <formula>AND(TODAY()-ROUNDDOWN(I2,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(I2,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
final copy-paste bug fix
</commit_message>
<xml_diff>
--- a/Calibration_TMA_SOP Schedule_Master Form 101359 TODO.xlsx
+++ b/Calibration_TMA_SOP Schedule_Master Form 101359 TODO.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="79">
   <si>
     <t xml:space="preserve">Master Form 101359 Calibration, Verification, Standardization Schedule </t>
   </si>
@@ -214,6 +214,21 @@
     <t>Titrando 905</t>
   </si>
   <si>
+    <t>copper strip dimensions (10.5-14.5mm width, 1.5-3.2mm thick, 70-80mm length)</t>
+  </si>
+  <si>
+    <t>Quarterly</t>
+  </si>
+  <si>
+    <t>JB</t>
+  </si>
+  <si>
+    <t>Check ASTM Copper Strip Corrosion Standard Chart for Fading</t>
+  </si>
+  <si>
+    <t>annually</t>
+  </si>
+  <si>
     <t xml:space="preserve">Secondary Working Standard </t>
   </si>
   <si>
@@ -229,9 +244,6 @@
     <t>Air Flow 10 L/h</t>
   </si>
   <si>
-    <t>Quarterly</t>
-  </si>
-  <si>
     <t>6-place block</t>
   </si>
   <si>
@@ -259,14 +271,20 @@
     <t>quarterly</t>
   </si>
   <si>
-    <t>JB</t>
+    <t>0.0355 @ 40C</t>
+  </si>
+  <si>
+    <t>DA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.00000"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -298,16 +316,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -341,11 +372,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -390,23 +434,32 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="19">
+  <dxfs count="48">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -506,16 +559,6 @@
         <color rgb="FF9C0006"/>
       </font>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="9" tint="0.39997558519241921"/>
@@ -540,6 +583,320 @@
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="9" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1066,31 +1423,31 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="79.95" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:15" ht="79.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="18"/>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
       <c r="D3" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="E3" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="E3" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19">
+      <c r="F3" s="18"/>
+      <c r="G3" s="22">
         <v>42676</v>
       </c>
-      <c r="H3" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="I3" s="19">
+      <c r="H3" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="I3" s="21">
         <v>42706</v>
       </c>
       <c r="J3" s="19"/>
-      <c r="K3" s="20"/>
-      <c r="L3" s="20"/>
-      <c r="M3" s="21"/>
-      <c r="N3" s="21"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
+      <c r="M3" s="19"/>
+      <c r="N3" s="18"/>
       <c r="O3">
         <v>48</v>
       </c>
@@ -1099,12 +1456,20 @@
   <mergeCells count="1">
     <mergeCell ref="A1:O1"/>
   </mergeCells>
-  <conditionalFormatting sqref="I2:I3">
-    <cfRule type="timePeriod" dxfId="12" priority="1" timePeriod="nextWeek">
+  <conditionalFormatting sqref="I2">
+    <cfRule type="timePeriod" dxfId="32" priority="3" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(I2,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(I2,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="11" priority="2" timePeriod="thisWeek">
+    <cfRule type="timePeriod" dxfId="31" priority="4" timePeriod="thisWeek">
       <formula>AND(TODAY()-ROUNDDOWN(I2,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(I2,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I3">
+    <cfRule type="timePeriod" dxfId="30" priority="1" timePeriod="nextWeek">
+      <formula>AND(ROUNDDOWN(I3,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(I3,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
+    </cfRule>
+    <cfRule type="timePeriod" dxfId="29" priority="2" timePeriod="thisWeek">
+      <formula>AND(TODAY()-ROUNDDOWN(I3,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(I3,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1113,7 +1478,7 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
@@ -1203,21 +1568,95 @@
         <v>10</v>
       </c>
     </row>
+    <row r="3" spans="1:15" s="8" customFormat="1" ht="79.95" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="18"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F3" s="18"/>
+      <c r="G3" s="22">
+        <v>42621</v>
+      </c>
+      <c r="H3" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="I3" s="21">
+        <v>42712</v>
+      </c>
+      <c r="J3" s="18"/>
+      <c r="K3"/>
+      <c r="L3"/>
+      <c r="M3" s="19"/>
+      <c r="N3" s="19"/>
+      <c r="O3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" s="8" customFormat="1" ht="79.95" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="18"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="F4" s="18"/>
+      <c r="G4" s="22">
+        <v>42621</v>
+      </c>
+      <c r="H4" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="I4" s="21">
+        <v>42712</v>
+      </c>
+      <c r="J4" s="18"/>
+      <c r="K4"/>
+      <c r="L4"/>
+      <c r="M4" s="19"/>
+      <c r="N4" s="19"/>
+      <c r="O4">
+        <v>49</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:O1"/>
   </mergeCells>
   <conditionalFormatting sqref="I2">
-    <cfRule type="timePeriod" dxfId="10" priority="2" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="28" priority="6" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(I2,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(I2,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="9" priority="3" timePeriod="thisWeek">
+    <cfRule type="timePeriod" dxfId="27" priority="7" timePeriod="thisWeek">
       <formula>AND(TODAY()-ROUNDDOWN(I2,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(I2,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2">
-    <cfRule type="timePeriod" dxfId="8" priority="1" timePeriod="nextMonth">
+    <cfRule type="timePeriod" dxfId="26" priority="5" timePeriod="nextMonth">
       <formula>AND(MONTH(I2)=MONTH(EDATE(TODAY(),0+1)),YEAR(I2)=YEAR(EDATE(TODAY(),0+1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I4">
+    <cfRule type="timePeriod" dxfId="25" priority="3" timePeriod="nextWeek">
+      <formula>AND(ROUNDDOWN(I4,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(I4,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
+    </cfRule>
+    <cfRule type="timePeriod" dxfId="24" priority="4" timePeriod="thisWeek">
+      <formula>AND(TODAY()-ROUNDDOWN(I4,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(I4,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I3">
+    <cfRule type="timePeriod" dxfId="23" priority="1" timePeriod="nextWeek">
+      <formula>AND(ROUNDDOWN(I3,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(I3,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
+    </cfRule>
+    <cfRule type="timePeriod" dxfId="22" priority="2" timePeriod="thisWeek">
+      <formula>AND(TODAY()-ROUNDDOWN(I3,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(I3,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1315,235 +1754,235 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A3" s="18"/>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19" t="s">
+      <c r="B3" s="18"/>
+      <c r="C3" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="E3" s="19" t="s">
+      <c r="E3" s="18" t="s">
         <v>56</v>
       </c>
       <c r="F3" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="G3" s="19">
+      <c r="G3" s="22">
         <v>42692</v>
       </c>
-      <c r="H3" s="19" t="s">
+      <c r="H3" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="I3" s="19">
+      <c r="I3" s="21">
         <v>42706</v>
       </c>
-      <c r="J3" s="19"/>
-      <c r="K3" s="20"/>
-      <c r="L3" s="20"/>
-      <c r="M3" s="21"/>
-      <c r="N3" s="21"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
+      <c r="M3" s="19"/>
+      <c r="N3" s="18"/>
       <c r="O3">
         <v>233</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="46.8" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:15" ht="42" x14ac:dyDescent="0.4">
       <c r="A4" s="18"/>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="E4" s="19" t="s">
+      <c r="E4" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="F4" s="19" t="s">
+      <c r="F4" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="G4" s="19">
+      <c r="G4" s="21">
         <v>42681</v>
       </c>
-      <c r="H4" s="19" t="s">
+      <c r="H4" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="I4" s="19">
+      <c r="I4" s="21">
         <v>42711</v>
       </c>
-      <c r="J4" s="19"/>
-      <c r="K4" s="20"/>
-      <c r="L4" s="20"/>
-      <c r="M4" s="21" t="s">
+      <c r="J4" s="18"/>
+      <c r="K4" s="23"/>
+      <c r="L4" s="21"/>
+      <c r="M4" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="N4" s="21" t="s">
+      <c r="N4" s="18" t="s">
         <v>54</v>
       </c>
       <c r="O4">
         <v>223</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="46.8" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:15" ht="42" x14ac:dyDescent="0.4">
       <c r="A5" s="18"/>
-      <c r="B5" s="19"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19" t="s">
+      <c r="B5" s="18"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="E5" s="19" t="s">
+      <c r="E5" s="18" t="s">
         <v>44</v>
       </c>
       <c r="F5" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="G5" s="19">
+      <c r="G5" s="21">
         <v>42675</v>
       </c>
-      <c r="H5" s="19" t="s">
+      <c r="H5" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="I5" s="19">
+      <c r="I5" s="21">
         <v>42705</v>
       </c>
-      <c r="J5" s="19"/>
-      <c r="K5" s="20"/>
-      <c r="L5" s="20"/>
-      <c r="M5" s="21"/>
-      <c r="N5" s="21"/>
+      <c r="J5" s="18"/>
+      <c r="K5" s="18"/>
+      <c r="L5" s="18"/>
+      <c r="M5" s="19"/>
+      <c r="N5" s="18"/>
       <c r="O5">
         <v>175</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="46.8" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:15" ht="42" x14ac:dyDescent="0.4">
       <c r="A6" s="18"/>
-      <c r="B6" s="19"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19" t="s">
+      <c r="B6" s="18"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="E6" s="19" t="s">
+      <c r="E6" s="18" t="s">
         <v>44</v>
       </c>
       <c r="F6" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="G6" s="19">
+      <c r="G6" s="21">
         <v>42675</v>
       </c>
-      <c r="H6" s="19" t="s">
+      <c r="H6" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="I6" s="19">
+      <c r="I6" s="21">
         <v>42705</v>
       </c>
-      <c r="J6" s="19"/>
-      <c r="K6" s="20"/>
-      <c r="L6" s="20"/>
-      <c r="M6" s="21"/>
-      <c r="N6" s="21"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="18"/>
+      <c r="M6" s="19"/>
+      <c r="N6" s="18"/>
       <c r="O6">
         <v>172</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="46.8" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:15" ht="42" x14ac:dyDescent="0.4">
       <c r="A7" s="18"/>
-      <c r="B7" s="19"/>
-      <c r="C7" s="19"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="18"/>
       <c r="D7" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="E7" s="19" t="s">
+      <c r="E7" s="18" t="s">
         <v>40</v>
       </c>
       <c r="F7" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="G7" s="19">
+      <c r="G7" s="22">
         <v>42527</v>
       </c>
-      <c r="H7" s="19" t="s">
+      <c r="H7" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="I7" s="19">
+      <c r="I7" s="22">
         <v>42710</v>
       </c>
-      <c r="J7" s="19"/>
-      <c r="K7" s="20"/>
-      <c r="L7" s="20"/>
-      <c r="M7" s="21"/>
-      <c r="N7" s="21"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="18"/>
+      <c r="M7" s="19"/>
+      <c r="N7" s="18"/>
       <c r="O7">
         <v>138</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="46.8" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:15" ht="42" x14ac:dyDescent="0.4">
       <c r="A8" s="18"/>
-      <c r="B8" s="19"/>
-      <c r="C8" s="19" t="s">
+      <c r="B8" s="18"/>
+      <c r="C8" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="19" t="s">
+      <c r="D8" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="E8" s="19" t="s">
+      <c r="E8" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="F8" s="19"/>
-      <c r="G8" s="19">
+      <c r="F8" s="20"/>
+      <c r="G8" s="21">
         <v>42669</v>
       </c>
-      <c r="H8" s="19" t="s">
+      <c r="H8" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="I8" s="19">
+      <c r="I8" s="21">
         <v>42700</v>
       </c>
-      <c r="J8" s="19"/>
-      <c r="K8" s="20">
+      <c r="J8" s="18"/>
+      <c r="K8" s="22">
         <v>41982</v>
       </c>
-      <c r="L8" s="20">
+      <c r="L8" s="23">
         <v>42347</v>
       </c>
-      <c r="M8" s="21" t="s">
+      <c r="M8" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="N8" s="21" t="s">
+      <c r="N8" s="18" t="s">
         <v>38</v>
       </c>
       <c r="O8">
         <v>92</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A9" s="18"/>
-      <c r="B9" s="19"/>
-      <c r="C9" s="19"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="18"/>
       <c r="D9" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="E9" s="19" t="s">
+      <c r="E9" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="F9" s="19"/>
-      <c r="G9" s="19">
+      <c r="F9" s="20"/>
+      <c r="G9" s="21">
         <v>42669</v>
       </c>
-      <c r="H9" s="19" t="s">
+      <c r="H9" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="I9" s="19">
+      <c r="I9" s="21">
         <v>42700</v>
       </c>
-      <c r="J9" s="19"/>
-      <c r="K9" s="20"/>
-      <c r="L9" s="20"/>
-      <c r="M9" s="21"/>
-      <c r="N9" s="21"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="18"/>
+      <c r="L9" s="18"/>
+      <c r="M9" s="19"/>
+      <c r="N9" s="18"/>
       <c r="O9">
         <v>91</v>
       </c>
@@ -1552,12 +1991,68 @@
   <mergeCells count="1">
     <mergeCell ref="A1:O1"/>
   </mergeCells>
-  <conditionalFormatting sqref="I2:I9">
+  <conditionalFormatting sqref="I2">
+    <cfRule type="timePeriod" dxfId="21" priority="15" timePeriod="nextWeek">
+      <formula>AND(ROUNDDOWN(I2,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(I2,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
+    </cfRule>
+    <cfRule type="timePeriod" dxfId="20" priority="16" timePeriod="thisWeek">
+      <formula>AND(TODAY()-ROUNDDOWN(I2,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(I2,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I9">
+    <cfRule type="timePeriod" dxfId="19" priority="13" timePeriod="nextWeek">
+      <formula>AND(ROUNDDOWN(I9,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(I9,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
+    </cfRule>
+    <cfRule type="timePeriod" dxfId="18" priority="14" timePeriod="thisWeek">
+      <formula>AND(TODAY()-ROUNDDOWN(I9,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(I9,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I8">
+    <cfRule type="timePeriod" dxfId="17" priority="11" timePeriod="nextWeek">
+      <formula>AND(ROUNDDOWN(I8,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(I8,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
+    </cfRule>
+    <cfRule type="timePeriod" dxfId="16" priority="12" timePeriod="thisWeek">
+      <formula>AND(TODAY()-ROUNDDOWN(I8,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(I8,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I7">
+    <cfRule type="timePeriod" dxfId="15" priority="9" timePeriod="nextWeek">
+      <formula>AND(ROUNDDOWN(I7,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(I7,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
+    </cfRule>
+    <cfRule type="timePeriod" dxfId="14" priority="10" timePeriod="thisWeek">
+      <formula>AND(TODAY()-ROUNDDOWN(I7,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(I7,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I6">
+    <cfRule type="timePeriod" dxfId="13" priority="7" timePeriod="nextWeek">
+      <formula>AND(ROUNDDOWN(I6,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(I6,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
+    </cfRule>
+    <cfRule type="timePeriod" dxfId="12" priority="8" timePeriod="thisWeek">
+      <formula>AND(TODAY()-ROUNDDOWN(I6,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(I6,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I5">
+    <cfRule type="timePeriod" dxfId="11" priority="5" timePeriod="nextWeek">
+      <formula>AND(ROUNDDOWN(I5,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(I5,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
+    </cfRule>
+    <cfRule type="timePeriod" dxfId="10" priority="6" timePeriod="thisWeek">
+      <formula>AND(TODAY()-ROUNDDOWN(I5,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(I5,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I4">
+    <cfRule type="timePeriod" dxfId="9" priority="3" timePeriod="nextWeek">
+      <formula>AND(ROUNDDOWN(I4,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(I4,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
+    </cfRule>
+    <cfRule type="timePeriod" dxfId="8" priority="4" timePeriod="thisWeek">
+      <formula>AND(TODAY()-ROUNDDOWN(I4,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(I4,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I3">
     <cfRule type="timePeriod" dxfId="7" priority="1" timePeriod="nextWeek">
-      <formula>AND(ROUNDDOWN(I2,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(I2,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
+      <formula>AND(ROUNDDOWN(I3,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(I3,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
     <cfRule type="timePeriod" dxfId="6" priority="2" timePeriod="thisWeek">
-      <formula>AND(TODAY()-ROUNDDOWN(I2,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(I2,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
+      <formula>AND(TODAY()-ROUNDDOWN(I3,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(I3,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2086,10 +2581,10 @@
     <mergeCell ref="A1:J1"/>
   </mergeCells>
   <conditionalFormatting sqref="I1">
-    <cfRule type="timePeriod" dxfId="18" priority="1" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="47" priority="1" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(I1,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(I1,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="17" priority="2" timePeriod="thisWeek">
+    <cfRule type="timePeriod" dxfId="46" priority="2" timePeriod="thisWeek">
       <formula>AND(TODAY()-ROUNDDOWN(I1,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(I1,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2099,7 +2594,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
@@ -2161,6 +2656,33 @@
       <c r="K2" s="4" t="s">
         <v>25</v>
       </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="27">
+        <v>150</v>
+      </c>
+      <c r="B3" s="27">
+        <v>1149</v>
+      </c>
+      <c r="C3" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="D3" s="29">
+        <v>42346</v>
+      </c>
+      <c r="E3" s="27" t="s">
+        <v>78</v>
+      </c>
+      <c r="F3" s="30"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="29">
+        <v>42712</v>
+      </c>
+      <c r="I3" s="32"/>
+      <c r="J3" s="10">
+        <v>108</v>
+      </c>
+      <c r="K3" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2272,10 +2794,10 @@
     <mergeCell ref="A1:P1"/>
   </mergeCells>
   <conditionalFormatting sqref="I2">
-    <cfRule type="timePeriod" dxfId="16" priority="1" timePeriod="nextWeek">
+    <cfRule type="timePeriod" dxfId="45" priority="1" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(I2,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(I2,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="15" priority="2" timePeriod="thisWeek">
+    <cfRule type="timePeriod" dxfId="44" priority="2" timePeriod="thisWeek">
       <formula>AND(TODAY()-ROUNDDOWN(I2,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(I2,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2374,31 +2896,31 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="93.6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:15" ht="63" x14ac:dyDescent="0.4">
       <c r="A3" s="18"/>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
       <c r="D3" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="E3" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19">
+        <v>75</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="F3" s="18"/>
+      <c r="G3" s="22">
         <v>42614</v>
       </c>
-      <c r="H3" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="I3" s="19">
+      <c r="H3" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="I3" s="21">
         <v>42705</v>
       </c>
-      <c r="J3" s="19"/>
-      <c r="K3" s="20"/>
-      <c r="L3" s="20"/>
-      <c r="M3" s="21"/>
-      <c r="N3" s="21"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="25"/>
+      <c r="L3" s="18"/>
+      <c r="M3" s="26"/>
+      <c r="N3" s="19"/>
       <c r="O3">
         <v>54</v>
       </c>
@@ -2407,6 +2929,19 @@
   <mergeCells count="1">
     <mergeCell ref="A1:O1"/>
   </mergeCells>
+  <conditionalFormatting sqref="I3">
+    <cfRule type="timePeriod" dxfId="43" priority="2" timePeriod="nextWeek">
+      <formula>AND(ROUNDDOWN(I3,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(I3,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
+    </cfRule>
+    <cfRule type="timePeriod" dxfId="42" priority="3" timePeriod="thisWeek">
+      <formula>AND(TODAY()-ROUNDDOWN(I3,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(I3,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I3">
+    <cfRule type="timePeriod" dxfId="41" priority="1" timePeriod="nextMonth">
+      <formula>AND(MONTH(I3)=MONTH(EDATE(TODAY(),0+1)),YEAR(I3)=YEAR(EDATE(TODAY(),0+1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2500,110 +3035,110 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="46.8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A3" s="18"/>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19" t="s">
-        <v>70</v>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18" t="s">
+        <v>74</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="E3" s="19" t="s">
-        <v>63</v>
-      </c>
-      <c r="F3" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="G3" s="19">
+        <v>67</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="F3" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="G3" s="22">
         <v>42619</v>
       </c>
-      <c r="H3" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="I3" s="19">
+      <c r="H3" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="I3" s="22">
         <v>42710</v>
       </c>
-      <c r="J3" s="19"/>
-      <c r="K3" s="20"/>
-      <c r="L3" s="20"/>
-      <c r="M3" s="21"/>
-      <c r="N3" s="21"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="22"/>
+      <c r="L3" s="22"/>
+      <c r="M3" s="18"/>
+      <c r="N3" s="18"/>
       <c r="O3">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="70.2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:15" ht="42" x14ac:dyDescent="0.4">
       <c r="A4" s="18"/>
-      <c r="B4" s="19"/>
+      <c r="B4" s="18"/>
       <c r="C4" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="F4" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="G4" s="22">
+        <v>42619</v>
+      </c>
+      <c r="H4" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="E4" s="19" t="s">
-        <v>63</v>
-      </c>
-      <c r="F4" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="G4" s="19">
-        <v>42619</v>
-      </c>
-      <c r="H4" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="I4" s="19">
+      <c r="I4" s="22">
         <v>42710</v>
       </c>
-      <c r="J4" s="19"/>
-      <c r="K4" s="20"/>
-      <c r="L4" s="20"/>
-      <c r="M4" s="21"/>
-      <c r="N4" s="21"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="22"/>
+      <c r="L4" s="22"/>
+      <c r="M4" s="18"/>
+      <c r="N4" s="18"/>
       <c r="O4">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="70.2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:15" ht="42" x14ac:dyDescent="0.4">
       <c r="A5" s="18"/>
-      <c r="B5" s="19" t="s">
-        <v>60</v>
+      <c r="B5" s="18" t="s">
+        <v>65</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="E5" s="19" t="s">
-        <v>63</v>
-      </c>
-      <c r="F5" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="G5" s="19">
+        <v>67</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="F5" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="G5" s="22">
         <v>42619</v>
       </c>
-      <c r="H5" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="I5" s="19">
+      <c r="H5" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="I5" s="22">
         <v>42710</v>
       </c>
-      <c r="J5" s="19"/>
-      <c r="K5" s="20">
+      <c r="J5" s="18"/>
+      <c r="K5" s="24">
         <v>42064</v>
       </c>
-      <c r="L5" s="20">
+      <c r="L5" s="23">
         <v>42430</v>
       </c>
-      <c r="M5" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="N5" s="21" t="s">
-        <v>67</v>
+      <c r="M5" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="N5" s="18" t="s">
+        <v>71</v>
       </c>
       <c r="O5">
         <v>1</v>
@@ -2613,12 +3148,36 @@
   <mergeCells count="1">
     <mergeCell ref="A1:O1"/>
   </mergeCells>
-  <conditionalFormatting sqref="I2:I5">
-    <cfRule type="timePeriod" dxfId="14" priority="1" timePeriod="nextWeek">
+  <conditionalFormatting sqref="I2">
+    <cfRule type="timePeriod" dxfId="40" priority="7" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(I2,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(I2,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="13" priority="2" timePeriod="thisWeek">
+    <cfRule type="timePeriod" dxfId="39" priority="8" timePeriod="thisWeek">
       <formula>AND(TODAY()-ROUNDDOWN(I2,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(I2,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I5">
+    <cfRule type="timePeriod" dxfId="38" priority="5" timePeriod="nextWeek">
+      <formula>AND(ROUNDDOWN(I5,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(I5,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
+    </cfRule>
+    <cfRule type="timePeriod" dxfId="37" priority="6" timePeriod="thisWeek">
+      <formula>AND(TODAY()-ROUNDDOWN(I5,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(I5,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I4">
+    <cfRule type="timePeriod" dxfId="36" priority="3" timePeriod="nextWeek">
+      <formula>AND(ROUNDDOWN(I4,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(I4,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
+    </cfRule>
+    <cfRule type="timePeriod" dxfId="35" priority="4" timePeriod="thisWeek">
+      <formula>AND(TODAY()-ROUNDDOWN(I4,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(I4,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I3">
+    <cfRule type="timePeriod" dxfId="34" priority="1" timePeriod="nextWeek">
+      <formula>AND(ROUNDDOWN(I3,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(I3,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
+    </cfRule>
+    <cfRule type="timePeriod" dxfId="33" priority="2" timePeriod="thisWeek">
+      <formula>AND(TODAY()-ROUNDDOWN(I3,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(I3,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>